<commit_message>
Java Excel file updated
</commit_message>
<xml_diff>
--- a/Java Documentation/Work status.xlsx
+++ b/Java Documentation/Work status.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\HiveEd\Notes\Java Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28FC2C7-CF5A-490F-81EC-C918AE1CC280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E701DD9-0EA8-4796-9D2C-095B65832391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{40566AF3-1D91-4421-8706-5B6838EDC1A0}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
-  <si>
-    <t>Java Tutorial</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>What is Java</t>
   </si>
@@ -51,12 +48,6 @@
     <t>krinishaa</t>
   </si>
   <si>
-    <t>document</t>
-  </si>
-  <si>
-    <t>git</t>
-  </si>
-  <si>
     <t>done</t>
   </si>
   <si>
@@ -73,6 +64,18 @@
   </si>
   <si>
     <t xml:space="preserve">scanner </t>
+  </si>
+  <si>
+    <t>work done by</t>
+  </si>
+  <si>
+    <t>document status</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>Concept</t>
   </si>
 </sst>
 </file>
@@ -426,81 +429,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFEFB992-FDAE-406D-8BCE-24F286EF6F81}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>